<commit_message>
Updating wing stuff and getting started with STACKS
Updating wing results to send to Giovan
Started stacks, working with kevin, making popmaps and doing alignments
</commit_message>
<xml_diff>
--- a/Gomez analysis plan/2017_09_06 Field 18 allometry table.xlsx
+++ b/Gomez analysis plan/2017_09_06 Field 18 allometry table.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vmc04\Documents\GitHub\wingproj\Gomez analysis plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\virgc\GitHub\wingproj\Gomez analysis plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21255" windowHeight="11850"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21255" windowHeight="11850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="62">
   <si>
     <t>Field 18 allometry</t>
   </si>
@@ -120,12 +120,102 @@
   </si>
   <si>
     <t>assignement</t>
+  </si>
+  <si>
+    <t>redid pad on 11/12/17</t>
+  </si>
+  <si>
+    <t>Cross Checked Classification</t>
+  </si>
+  <si>
+    <t>First Correct attributions</t>
+  </si>
+  <si>
+    <t>------------------------</t>
+  </si>
+  <si>
+    <t>Pop 1 : 5 / 17</t>
+  </si>
+  <si>
+    <t>Pop 2 : 17 / 50</t>
+  </si>
+  <si>
+    <t>Pop 3 : 32 / 47</t>
+  </si>
+  <si>
+    <t>Pop 4 : 23 / 45</t>
+  </si>
+  <si>
+    <t>Pop 5 : 43 / 54</t>
+  </si>
+  <si>
+    <t>Pop 6 : 10 / 17</t>
+  </si>
+  <si>
+    <t>Pop 7 : 7 / 11</t>
+  </si>
+  <si>
+    <t>Simple re-classification</t>
+  </si>
+  <si>
+    <t>First Correct assignement</t>
+  </si>
+  <si>
+    <t>Pop 1 :  12 / 17</t>
+  </si>
+  <si>
+    <t>Pop 2 :  31 / 50</t>
+  </si>
+  <si>
+    <t>Pop 3 :  41 / 47</t>
+  </si>
+  <si>
+    <t>Pop 4 :  30 / 45</t>
+  </si>
+  <si>
+    <t>Pop 5 :  46 / 54</t>
+  </si>
+  <si>
+    <t>Pop 6 :  16 / 17</t>
+  </si>
+  <si>
+    <t>Pop 7 :  10 / 11</t>
+  </si>
+  <si>
+    <t>Cross check</t>
+  </si>
+  <si>
+    <t>5/17</t>
+  </si>
+  <si>
+    <t>17/50</t>
+  </si>
+  <si>
+    <t>32/47</t>
+  </si>
+  <si>
+    <t>23/45</t>
+  </si>
+  <si>
+    <t>7/11</t>
+  </si>
+  <si>
+    <t>43/54</t>
+  </si>
+  <si>
+    <t>10/17</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>1st correct assignment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -151,7 +241,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -159,17 +249,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,19 +596,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15:I23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="7" max="7" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.19921875" customWidth="1"/>
+    <col min="7" max="7" width="20.73046875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.796875" customWidth="1"/>
+    <col min="13" max="13" width="10.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -503,12 +619,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C3" t="s">
         <v>8</v>
       </c>
@@ -516,7 +632,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -533,7 +649,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
@@ -550,7 +666,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -567,7 +683,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
@@ -584,7 +700,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
         <v>5</v>
       </c>
@@ -601,7 +717,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
         <v>6</v>
       </c>
@@ -618,7 +734,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
         <v>7</v>
       </c>
@@ -635,12 +751,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -651,7 +767,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B16" t="s">
         <v>1</v>
       </c>
@@ -664,7 +780,7 @@
       <c r="G16" s="5"/>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B17" s="3" t="s">
         <v>2</v>
       </c>
@@ -677,7 +793,7 @@
       <c r="F17" s="3"/>
       <c r="H17" s="4"/>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B18" t="s">
         <v>3</v>
       </c>
@@ -689,7 +805,7 @@
       </c>
       <c r="H18" s="4"/>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B19" s="3" t="s">
         <v>4</v>
       </c>
@@ -702,7 +818,7 @@
       <c r="F19" s="3"/>
       <c r="H19" s="4"/>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
         <v>5</v>
       </c>
@@ -714,7 +830,7 @@
       </c>
       <c r="H20" s="4"/>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B21" t="s">
         <v>6</v>
       </c>
@@ -726,7 +842,7 @@
       </c>
       <c r="H21" s="4"/>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B22" t="s">
         <v>7</v>
       </c>
@@ -739,7 +855,258 @@
       <c r="G22" s="5"/>
       <c r="H22" s="4"/>
     </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="B25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G25" t="s">
+        <v>33</v>
+      </c>
+      <c r="K25" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="L25" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="M25" s="7"/>
+      <c r="N25" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="O25" s="7"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="B26" t="s">
+        <v>44</v>
+      </c>
+      <c r="G26" t="s">
+        <v>34</v>
+      </c>
+      <c r="K26" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L26" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M26" s="9">
+        <v>0.7</v>
+      </c>
+      <c r="N26" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="O26" s="9">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="K27" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="L27" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="M27" s="9">
+        <v>0.62</v>
+      </c>
+      <c r="N27" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="O27" s="9">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="B28" t="s">
+        <v>35</v>
+      </c>
+      <c r="G28" t="s">
+        <v>35</v>
+      </c>
+      <c r="K28" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="L28" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M28" s="9">
+        <v>0.87</v>
+      </c>
+      <c r="N28" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="O28" s="9">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="K29" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="L29" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="M29" s="9">
+        <v>0.66</v>
+      </c>
+      <c r="N29" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="O29" s="9">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="B30" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30" s="4">
+        <v>-0.7</v>
+      </c>
+      <c r="G30" t="s">
+        <v>36</v>
+      </c>
+      <c r="H30" s="4">
+        <v>-0.28999999999999998</v>
+      </c>
+      <c r="K30" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="L30" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="M30" s="9">
+        <v>0.85</v>
+      </c>
+      <c r="N30" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="O30" s="9">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="B31" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" s="4">
+        <v>-0.62</v>
+      </c>
+      <c r="G31" t="s">
+        <v>37</v>
+      </c>
+      <c r="H31" s="4">
+        <v>-0.34</v>
+      </c>
+      <c r="K31" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L31" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="M31" s="9">
+        <v>0.94</v>
+      </c>
+      <c r="N31" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="O31" s="9">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="B32" t="s">
+        <v>47</v>
+      </c>
+      <c r="C32" s="4">
+        <v>-0.87</v>
+      </c>
+      <c r="G32" t="s">
+        <v>38</v>
+      </c>
+      <c r="H32" s="4">
+        <v>-0.68</v>
+      </c>
+      <c r="K32" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="L32" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M32" s="9">
+        <v>0.9</v>
+      </c>
+      <c r="N32" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="O32" s="9">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B33" t="s">
+        <v>48</v>
+      </c>
+      <c r="C33" s="4">
+        <v>-0.66</v>
+      </c>
+      <c r="G33" t="s">
+        <v>39</v>
+      </c>
+      <c r="H33" s="4">
+        <v>-0.51</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B34" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" s="4">
+        <v>-0.85</v>
+      </c>
+      <c r="G34" t="s">
+        <v>40</v>
+      </c>
+      <c r="H34" s="4">
+        <v>-0.79</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B35" t="s">
+        <v>50</v>
+      </c>
+      <c r="C35" s="4">
+        <v>-0.94</v>
+      </c>
+      <c r="G35" t="s">
+        <v>41</v>
+      </c>
+      <c r="H35" s="4">
+        <v>-0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B36" t="s">
+        <v>51</v>
+      </c>
+      <c r="C36" s="4">
+        <v>-0.9</v>
+      </c>
+      <c r="G36" t="s">
+        <v>42</v>
+      </c>
+      <c r="H36" s="4">
+        <v>-0.63</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="N25:O25"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>